<commit_message>
converting URIs into w3id.org/italia/controlled-vocabulary for poi-category controlled vocabulary and inserted German translations of the labels in all its formats
</commit_message>
<xml_diff>
--- a/VocabolariControllati/poi-category-classification/poi-category.xlsx
+++ b/VocabolariControllati/poi-category-classification/poi-category.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Codice</t>
-  </si>
-  <si>
-    <t>Primo Livello</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>cat_1</t>
   </si>
@@ -73,18 +67,79 @@
   </si>
   <si>
     <t>Settore altri servizi pubblici</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Unterhaltungssektor</t>
+  </si>
+  <si>
+    <t>Leisure</t>
+  </si>
+  <si>
+    <t>Freizeitssektor</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Lebensmittelsektor</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Einkaufssektor</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Automobilsektor</t>
+  </si>
+  <si>
+    <t>Travel/Tourism</t>
+  </si>
+  <si>
+    <t>Reise-/Tourismussektor</t>
+  </si>
+  <si>
+    <t>Geographical</t>
+  </si>
+  <si>
+    <t>Geographischer Sektor</t>
+  </si>
+  <si>
+    <t>Other public services</t>
+  </si>
+  <si>
+    <t>Sonstige öffentliche Dienstleistungen</t>
+  </si>
+  <si>
+    <t>codice_1_livello</t>
+  </si>
+  <si>
+    <t>label_ITA_1_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_1_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_1_livello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,6 +166,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,9 +194,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
@@ -470,87 +531,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B11"/>
+  <dimension ref="A3:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>